<commit_message>
Issue#25 Req 5.1  update: back to basics of using apachePOI ------------------------------------------------------------------------  false green unit 6.1.2 - check if age for Unified Model is converted properly  this is false due to fact that application works only when excel date format  is set to dd-mm-yyyy
</commit_message>
<xml_diff>
--- a/SAP_age_conversion_check.xlsx
+++ b/SAP_age_conversion_check.xlsx
@@ -137,7 +137,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -654,7 +654,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -981,7 +981,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Issue#25 Req 5.1  Green Unit 6.1.2 - check if age for Unified Model is converted properly
</commit_message>
<xml_diff>
--- a/SAP_age_conversion_check.xlsx
+++ b/SAP_age_conversion_check.xlsx
@@ -136,9 +136,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy"/>
-  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -640,7 +637,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -654,9 +651,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -981,7 +975,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1075,7 +1069,7 @@
       <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="5">
         <v>30582</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -1116,7 +1110,7 @@
       <c r="K3" s="4">
         <v>664422</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="5">
         <v>33504</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -1157,7 +1151,7 @@
       <c r="K4" s="4">
         <v>600334</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="5">
         <v>28756</v>
       </c>
       <c r="M4" s="4" t="s">

</xml_diff>